<commit_message>
add permissions to data in search and fix code in import screens
</commit_message>
<xml_diff>
--- a/sql/sections.xlsx
+++ b/sql/sections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>nameAr</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -365,38 +368,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>